<commit_message>
feature: Add Algorithm to find available people
</commit_message>
<xml_diff>
--- a/SampleData/02_Anwesenheit/Urlaubs-Schulkalender_23.xlsx
+++ b/SampleData/02_Anwesenheit/Urlaubs-Schulkalender_23.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Zentral\Ausbildung\02_Anwesenheit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrick/dev/Web Projects/MurrChooser/SampleData/02_Anwesenheit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D288891-5563-4B66-BE1C-32DF210B51C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A3E5C2-1C92-9648-BE8A-62B1E8AE2F5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Januar Februar 2023" sheetId="8" r:id="rId1"/>
@@ -626,7 +626,7 @@
     <numFmt numFmtId="164" formatCode="[$-407]mmmm\ yy;@"/>
     <numFmt numFmtId="165" formatCode="dd"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1368,30 +1368,30 @@
       <selection pane="bottomRight" activeCell="A33" sqref="A33:XFD33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" customWidth="1"/>
     <col min="5" max="5" width="3" customWidth="1"/>
-    <col min="6" max="6" width="3.42578125" customWidth="1"/>
+    <col min="6" max="6" width="3.5" customWidth="1"/>
     <col min="7" max="14" width="3" customWidth="1"/>
-    <col min="15" max="15" width="3.28515625" customWidth="1"/>
+    <col min="15" max="15" width="3.33203125" customWidth="1"/>
     <col min="16" max="18" width="3" customWidth="1"/>
-    <col min="19" max="21" width="3.28515625" customWidth="1"/>
-    <col min="22" max="22" width="3.42578125" customWidth="1"/>
-    <col min="23" max="34" width="3.28515625" customWidth="1"/>
+    <col min="19" max="21" width="3.33203125" customWidth="1"/>
+    <col min="22" max="22" width="3.5" customWidth="1"/>
+    <col min="23" max="34" width="3.33203125" customWidth="1"/>
     <col min="35" max="36" width="3" customWidth="1"/>
-    <col min="37" max="38" width="3.28515625" customWidth="1"/>
+    <col min="37" max="38" width="3.33203125" customWidth="1"/>
     <col min="39" max="39" width="4" customWidth="1"/>
-    <col min="40" max="50" width="3.28515625" customWidth="1"/>
+    <col min="40" max="50" width="3.33203125" customWidth="1"/>
     <col min="51" max="56" width="3" customWidth="1"/>
-    <col min="57" max="57" width="3.28515625" customWidth="1"/>
+    <col min="57" max="57" width="3.33203125" customWidth="1"/>
     <col min="58" max="63" width="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:63">
       <c r="A1" s="41" t="s">
         <v>25</v>
       </c>
@@ -1458,7 +1458,7 @@
       <c r="BJ1" s="6"/>
       <c r="BK1" s="6"/>
     </row>
-    <row r="2" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:63">
       <c r="A2" s="41"/>
       <c r="B2" s="41"/>
       <c r="C2" s="41"/>
@@ -1549,7 +1549,7 @@
       <c r="BJ2" s="6"/>
       <c r="BK2" s="6"/>
     </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:63">
       <c r="A3" s="41"/>
       <c r="B3" s="41"/>
       <c r="C3" s="41"/>
@@ -1640,7 +1640,7 @@
       <c r="BJ3" s="6"/>
       <c r="BK3" s="6"/>
     </row>
-    <row r="4" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:63">
       <c r="A4" s="23"/>
       <c r="B4" s="23"/>
       <c r="C4" s="23"/>
@@ -1717,7 +1717,7 @@
       <c r="BJ4" s="6"/>
       <c r="BK4" s="6"/>
     </row>
-    <row r="6" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:63">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -1788,7 +1788,7 @@
       <c r="BJ6" s="43"/>
       <c r="BK6" s="43"/>
     </row>
-    <row r="7" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:63">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -1979,7 +1979,7 @@
         <v>44497</v>
       </c>
     </row>
-    <row r="8" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:63">
       <c r="A8" s="44" t="s">
         <v>5</v>
       </c>
@@ -2050,7 +2050,7 @@
       <c r="BJ8" s="26"/>
       <c r="BK8" s="26"/>
     </row>
-    <row r="9" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:63">
       <c r="A9" s="5" t="s">
         <v>113</v>
       </c>
@@ -2145,7 +2145,7 @@
       <c r="BJ9" s="26"/>
       <c r="BK9" s="26"/>
     </row>
-    <row r="10" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:63">
       <c r="A10" s="5" t="s">
         <v>115</v>
       </c>
@@ -2244,7 +2244,7 @@
       <c r="BJ10" s="26"/>
       <c r="BK10" s="26"/>
     </row>
-    <row r="11" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:63">
       <c r="A11" s="5" t="s">
         <v>117</v>
       </c>
@@ -2345,7 +2345,7 @@
       <c r="BJ11" s="26"/>
       <c r="BK11" s="26"/>
     </row>
-    <row r="12" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:63">
       <c r="A12" s="5" t="s">
         <v>119</v>
       </c>
@@ -2454,7 +2454,7 @@
       <c r="BJ12" s="26"/>
       <c r="BK12" s="26"/>
     </row>
-    <row r="13" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:63">
       <c r="A13" s="5" t="s">
         <v>121</v>
       </c>
@@ -2557,7 +2557,7 @@
       <c r="BJ13" s="26"/>
       <c r="BK13" s="26"/>
     </row>
-    <row r="14" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:63">
       <c r="A14" s="5" t="s">
         <v>94</v>
       </c>
@@ -2660,7 +2660,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:63">
       <c r="A15" s="5" t="s">
         <v>96</v>
       </c>
@@ -2763,7 +2763,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:63">
       <c r="A16" s="5" t="s">
         <v>90</v>
       </c>
@@ -2854,7 +2854,7 @@
       <c r="BJ16" s="26"/>
       <c r="BK16" s="26"/>
     </row>
-    <row r="17" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:63">
       <c r="A17" s="5" t="s">
         <v>92</v>
       </c>
@@ -2945,7 +2945,7 @@
       <c r="BJ17" s="26"/>
       <c r="BK17" s="26"/>
     </row>
-    <row r="18" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:63">
       <c r="A18" s="5" t="s">
         <v>53</v>
       </c>
@@ -3036,7 +3036,7 @@
       <c r="BJ18" s="26"/>
       <c r="BK18" s="26"/>
     </row>
-    <row r="19" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:63">
       <c r="A19" s="5" t="s">
         <v>180</v>
       </c>
@@ -3153,7 +3153,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="20" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:63">
       <c r="A20" s="5" t="s">
         <v>57</v>
       </c>
@@ -3252,7 +3252,7 @@
       <c r="BJ20" s="26"/>
       <c r="BK20" s="26"/>
     </row>
-    <row r="21" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:63">
       <c r="A21" s="5" t="s">
         <v>55</v>
       </c>
@@ -3357,7 +3357,7 @@
       <c r="BJ21" s="26"/>
       <c r="BK21" s="26"/>
     </row>
-    <row r="22" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:63">
       <c r="A22" s="5" t="s">
         <v>6</v>
       </c>
@@ -3440,7 +3440,7 @@
       <c r="BJ22" s="50"/>
       <c r="BK22" s="51"/>
     </row>
-    <row r="23" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:63">
       <c r="A23" s="5" t="s">
         <v>8</v>
       </c>
@@ -3523,7 +3523,7 @@
       <c r="BJ23" s="50"/>
       <c r="BK23" s="51"/>
     </row>
-    <row r="24" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:63">
       <c r="A24" s="5" t="s">
         <v>10</v>
       </c>
@@ -3606,7 +3606,7 @@
       <c r="BJ24" s="50"/>
       <c r="BK24" s="51"/>
     </row>
-    <row r="25" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:63">
       <c r="A25" s="5" t="s">
         <v>123</v>
       </c>
@@ -3713,7 +3713,7 @@
       </c>
       <c r="BK25" s="26"/>
     </row>
-    <row r="26" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:63">
       <c r="A26" s="5" t="s">
         <v>124</v>
       </c>
@@ -3824,7 +3824,7 @@
       </c>
       <c r="BK26" s="26"/>
     </row>
-    <row r="27" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:63">
       <c r="A27" s="5" t="s">
         <v>125</v>
       </c>
@@ -3927,7 +3927,7 @@
       </c>
       <c r="BK27" s="26"/>
     </row>
-    <row r="28" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:63">
       <c r="A28" s="5" t="s">
         <v>127</v>
       </c>
@@ -4046,7 +4046,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:63">
       <c r="A29" s="5" t="s">
         <v>88</v>
       </c>
@@ -4119,7 +4119,7 @@
       <c r="BJ29" s="26"/>
       <c r="BK29" s="26"/>
     </row>
-    <row r="30" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:63">
       <c r="A30" s="5" t="s">
         <v>59</v>
       </c>
@@ -4208,7 +4208,7 @@
       <c r="BJ30" s="26"/>
       <c r="BK30" s="26"/>
     </row>
-    <row r="31" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:63">
       <c r="A31" s="5" t="s">
         <v>61</v>
       </c>
@@ -4289,7 +4289,7 @@
       <c r="BJ31" s="26"/>
       <c r="BK31" s="26"/>
     </row>
-    <row r="32" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:63">
       <c r="A32" s="5" t="s">
         <v>130</v>
       </c>
@@ -4400,7 +4400,7 @@
       <c r="BJ32" s="26"/>
       <c r="BK32" s="26"/>
     </row>
-    <row r="33" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:63">
       <c r="A33" s="5" t="s">
         <v>132</v>
       </c>
@@ -4503,7 +4503,7 @@
       <c r="BJ33" s="26"/>
       <c r="BK33" s="26"/>
     </row>
-    <row r="34" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:63">
       <c r="A34" s="5" t="s">
         <v>63</v>
       </c>
@@ -4600,7 +4600,7 @@
       </c>
       <c r="BK34" s="26"/>
     </row>
-    <row r="35" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:63">
       <c r="A35" s="5" t="s">
         <v>134</v>
       </c>
@@ -4691,7 +4691,7 @@
       <c r="BJ35" s="26"/>
       <c r="BK35" s="26"/>
     </row>
-    <row r="36" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:63">
       <c r="A36" s="5" t="s">
         <v>89</v>
       </c>
@@ -4788,7 +4788,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:63">
       <c r="A37" s="1" t="s">
         <v>13</v>
       </c>
@@ -4855,7 +4855,7 @@
       <c r="BJ37" s="40"/>
       <c r="BK37" s="40"/>
     </row>
-    <row r="38" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:63">
       <c r="A38" s="6" t="s">
         <v>146</v>
       </c>
@@ -5010,7 +5010,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:63">
       <c r="A39" s="6" t="s">
         <v>154</v>
       </c>
@@ -5157,7 +5157,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:63">
       <c r="A40" s="6" t="s">
         <v>98</v>
       </c>
@@ -5312,7 +5312,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:63">
       <c r="A41" s="6" t="s">
         <v>100</v>
       </c>
@@ -5467,7 +5467,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:63">
       <c r="A42" s="6" t="s">
         <v>102</v>
       </c>
@@ -5622,7 +5622,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:63">
       <c r="A43" s="6" t="s">
         <v>65</v>
       </c>
@@ -5695,7 +5695,7 @@
       <c r="BJ43" s="26"/>
       <c r="BK43" s="26"/>
     </row>
-    <row r="44" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:63">
       <c r="A44" s="6" t="s">
         <v>67</v>
       </c>
@@ -5836,7 +5836,7 @@
       <c r="BJ44" s="26"/>
       <c r="BK44" s="26"/>
     </row>
-    <row r="45" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:63">
       <c r="A45" s="6" t="s">
         <v>69</v>
       </c>
@@ -5977,7 +5977,7 @@
       <c r="BJ45" s="26"/>
       <c r="BK45" s="26"/>
     </row>
-    <row r="46" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:63">
       <c r="A46" s="6" t="s">
         <v>136</v>
       </c>
@@ -6058,7 +6058,7 @@
       <c r="BJ46" s="26"/>
       <c r="BK46" s="26"/>
     </row>
-    <row r="47" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:63">
       <c r="A47" s="6" t="s">
         <v>71</v>
       </c>
@@ -6209,7 +6209,7 @@
       <c r="BJ47" s="26"/>
       <c r="BK47" s="26"/>
     </row>
-    <row r="48" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:63">
       <c r="A48" s="6" t="s">
         <v>138</v>
       </c>
@@ -6364,7 +6364,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:63">
       <c r="A49" s="6" t="s">
         <v>139</v>
       </c>
@@ -6519,7 +6519,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:63">
       <c r="A50" s="6" t="s">
         <v>103</v>
       </c>
@@ -6674,7 +6674,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:63">
       <c r="A51" s="6" t="s">
         <v>141</v>
       </c>
@@ -6829,7 +6829,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:63">
       <c r="A52" s="6" t="s">
         <v>143</v>
       </c>
@@ -6984,7 +6984,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="53" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:63">
       <c r="A53" s="6" t="s">
         <v>73</v>
       </c>
@@ -7091,7 +7091,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="54" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:63">
       <c r="A54" s="6" t="s">
         <v>65</v>
       </c>
@@ -7188,7 +7188,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="55" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:63">
       <c r="A55" s="6" t="s">
         <v>144</v>
       </c>
@@ -7343,7 +7343,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="56" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:63">
       <c r="A56" s="1" t="s">
         <v>18</v>
       </c>
@@ -7410,7 +7410,7 @@
       <c r="BJ56" s="40"/>
       <c r="BK56" s="40"/>
     </row>
-    <row r="57" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:63">
       <c r="A57" s="6" t="s">
         <v>19</v>
       </c>
@@ -7491,7 +7491,7 @@
       <c r="BJ57" s="26"/>
       <c r="BK57" s="26"/>
     </row>
-    <row r="58" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:63">
       <c r="A58" s="6" t="s">
         <v>22</v>
       </c>
@@ -7574,7 +7574,7 @@
       <c r="BJ58" s="26"/>
       <c r="BK58" s="26"/>
     </row>
-    <row r="59" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:63">
       <c r="A59" s="6" t="s">
         <v>11</v>
       </c>
@@ -7657,7 +7657,7 @@
       </c>
       <c r="BK59" s="26"/>
     </row>
-    <row r="61" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:63">
       <c r="L61" s="27"/>
       <c r="R61" s="28"/>
       <c r="AR61" s="22" t="s">
@@ -7668,12 +7668,12 @@
       </c>
       <c r="AV61" s="27"/>
     </row>
-    <row r="62" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:63">
       <c r="AS62" s="6" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="63" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:63">
       <c r="BE63" s="22" t="s">
         <v>36</v>
       </c>
@@ -7681,7 +7681,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="64" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:63">
       <c r="BF64" s="6" t="s">
         <v>173</v>
       </c>
@@ -7719,35 +7719,35 @@
       <selection pane="bottomRight" activeCell="BO11" sqref="BO11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.85546875" customWidth="1"/>
+    <col min="6" max="6" width="2.83203125" customWidth="1"/>
     <col min="7" max="14" width="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="2.7109375" customWidth="1"/>
+    <col min="15" max="15" width="2.6640625" customWidth="1"/>
     <col min="16" max="21" width="3" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="3" customWidth="1"/>
     <col min="23" max="26" width="3" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="3.42578125" customWidth="1"/>
+    <col min="27" max="27" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="3.5" customWidth="1"/>
     <col min="29" max="37" width="3" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="2.85546875" customWidth="1"/>
+    <col min="38" max="38" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="2.83203125" customWidth="1"/>
     <col min="40" max="45" width="3" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="3.28515625" customWidth="1"/>
-    <col min="47" max="47" width="2.85546875" customWidth="1"/>
+    <col min="46" max="46" width="3.33203125" customWidth="1"/>
+    <col min="47" max="47" width="2.83203125" customWidth="1"/>
     <col min="48" max="56" width="3" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="2.7109375" customWidth="1"/>
+    <col min="57" max="57" width="2.6640625" customWidth="1"/>
     <col min="58" max="62" width="3" bestFit="1" customWidth="1"/>
     <col min="63" max="64" width="3" customWidth="1"/>
     <col min="65" max="65" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:65">
       <c r="A1" s="41" t="s">
         <v>25</v>
       </c>
@@ -7816,7 +7816,7 @@
       <c r="BL1" s="6"/>
       <c r="BM1" s="6"/>
     </row>
-    <row r="2" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:65">
       <c r="A2" s="41"/>
       <c r="B2" s="41"/>
       <c r="C2" s="41"/>
@@ -7909,7 +7909,7 @@
       <c r="BL2" s="6"/>
       <c r="BM2" s="6"/>
     </row>
-    <row r="3" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:65">
       <c r="A3" s="41"/>
       <c r="B3" s="41"/>
       <c r="C3" s="41"/>
@@ -8002,7 +8002,7 @@
       <c r="BL3" s="6"/>
       <c r="BM3" s="6"/>
     </row>
-    <row r="4" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:65">
       <c r="A4" s="23"/>
       <c r="B4" s="23"/>
       <c r="C4" s="23"/>
@@ -8081,7 +8081,7 @@
       <c r="BL4" s="6"/>
       <c r="BM4" s="6"/>
     </row>
-    <row r="6" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:65">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -8154,7 +8154,7 @@
       <c r="BL6" s="43"/>
       <c r="BM6" s="52"/>
     </row>
-    <row r="7" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:65">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -8351,7 +8351,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:65">
       <c r="A8" s="44" t="s">
         <v>5</v>
       </c>
@@ -8430,7 +8430,7 @@
       <c r="BL8" s="9"/>
       <c r="BM8" s="9"/>
     </row>
-    <row r="9" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:65">
       <c r="A9" s="5" t="s">
         <v>113</v>
       </c>
@@ -8527,7 +8527,7 @@
       <c r="BL9" s="9"/>
       <c r="BM9" s="9"/>
     </row>
-    <row r="10" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:65">
       <c r="A10" s="5" t="s">
         <v>115</v>
       </c>
@@ -8626,7 +8626,7 @@
       <c r="BL10" s="9"/>
       <c r="BM10" s="9"/>
     </row>
-    <row r="11" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:65">
       <c r="A11" s="5" t="s">
         <v>117</v>
       </c>
@@ -8739,7 +8739,7 @@
       <c r="BL11" s="9"/>
       <c r="BM11" s="9"/>
     </row>
-    <row r="12" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:65">
       <c r="A12" s="5" t="s">
         <v>119</v>
       </c>
@@ -8838,7 +8838,7 @@
       <c r="BL12" s="9"/>
       <c r="BM12" s="9"/>
     </row>
-    <row r="13" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:65">
       <c r="A13" s="5" t="s">
         <v>121</v>
       </c>
@@ -8943,7 +8943,7 @@
       <c r="BL13" s="9"/>
       <c r="BM13" s="9"/>
     </row>
-    <row r="14" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:65">
       <c r="A14" s="5" t="s">
         <v>94</v>
       </c>
@@ -9046,7 +9046,7 @@
       <c r="BL14" s="9"/>
       <c r="BM14" s="9"/>
     </row>
-    <row r="15" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:65">
       <c r="A15" s="5" t="s">
         <v>96</v>
       </c>
@@ -9151,7 +9151,7 @@
       <c r="BL15" s="9"/>
       <c r="BM15" s="9"/>
     </row>
-    <row r="16" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:65">
       <c r="A16" s="5" t="s">
         <v>90</v>
       </c>
@@ -9258,7 +9258,7 @@
       <c r="BL16" s="9"/>
       <c r="BM16" s="9"/>
     </row>
-    <row r="17" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:65">
       <c r="A17" s="5" t="s">
         <v>92</v>
       </c>
@@ -9367,7 +9367,7 @@
       <c r="BL17" s="9"/>
       <c r="BM17" s="9"/>
     </row>
-    <row r="18" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:65">
       <c r="A18" s="5" t="s">
         <v>53</v>
       </c>
@@ -9474,7 +9474,7 @@
       <c r="BL18" s="9"/>
       <c r="BM18" s="9"/>
     </row>
-    <row r="19" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:65">
       <c r="A19" s="5" t="s">
         <v>180</v>
       </c>
@@ -9603,7 +9603,7 @@
       <c r="BL19" s="9"/>
       <c r="BM19" s="9"/>
     </row>
-    <row r="20" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:65">
       <c r="A20" s="5" t="s">
         <v>57</v>
       </c>
@@ -9732,7 +9732,7 @@
       <c r="BL20" s="9"/>
       <c r="BM20" s="9"/>
     </row>
-    <row r="21" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:65">
       <c r="A21" s="5" t="s">
         <v>55</v>
       </c>
@@ -9827,7 +9827,7 @@
       <c r="BL21" s="9"/>
       <c r="BM21" s="9"/>
     </row>
-    <row r="22" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:65">
       <c r="A22" s="5" t="s">
         <v>123</v>
       </c>
@@ -9936,7 +9936,7 @@
       <c r="BL22" s="9"/>
       <c r="BM22" s="9"/>
     </row>
-    <row r="23" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:65">
       <c r="A23" s="5" t="s">
         <v>124</v>
       </c>
@@ -10043,7 +10043,7 @@
       <c r="BL23" s="9"/>
       <c r="BM23" s="9"/>
     </row>
-    <row r="24" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:65">
       <c r="A24" s="5" t="s">
         <v>125</v>
       </c>
@@ -10150,7 +10150,7 @@
       <c r="BL24" s="9"/>
       <c r="BM24" s="9"/>
     </row>
-    <row r="25" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:65">
       <c r="A25" s="5" t="s">
         <v>127</v>
       </c>
@@ -10263,7 +10263,7 @@
       <c r="BL25" s="9"/>
       <c r="BM25" s="9"/>
     </row>
-    <row r="26" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:65">
       <c r="A26" s="5" t="s">
         <v>88</v>
       </c>
@@ -10356,7 +10356,7 @@
       <c r="BL26" s="9"/>
       <c r="BM26" s="9"/>
     </row>
-    <row r="27" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:65">
       <c r="A27" s="5" t="s">
         <v>130</v>
       </c>
@@ -10465,7 +10465,7 @@
       <c r="BL27" s="9"/>
       <c r="BM27" s="9"/>
     </row>
-    <row r="28" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:65">
       <c r="A28" s="5" t="s">
         <v>132</v>
       </c>
@@ -10584,7 +10584,7 @@
       <c r="BL28" s="9"/>
       <c r="BM28" s="9"/>
     </row>
-    <row r="29" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:65">
       <c r="A29" s="5" t="s">
         <v>63</v>
       </c>
@@ -10715,7 +10715,7 @@
       <c r="BL29" s="9"/>
       <c r="BM29" s="9"/>
     </row>
-    <row r="30" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:65">
       <c r="A30" s="5" t="s">
         <v>134</v>
       </c>
@@ -10830,7 +10830,7 @@
       <c r="BL30" s="9"/>
       <c r="BM30" s="9"/>
     </row>
-    <row r="31" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:65">
       <c r="A31" s="5" t="s">
         <v>89</v>
       </c>
@@ -10943,7 +10943,7 @@
       <c r="BL31" s="9"/>
       <c r="BM31" s="9"/>
     </row>
-    <row r="32" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:65">
       <c r="A32" s="1" t="s">
         <v>13</v>
       </c>
@@ -11012,7 +11012,7 @@
       <c r="BL32" s="40"/>
       <c r="BM32" s="40"/>
     </row>
-    <row r="33" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:65">
       <c r="A33" s="6" t="s">
         <v>146</v>
       </c>
@@ -11135,7 +11135,7 @@
       <c r="BL33" s="9"/>
       <c r="BM33" s="9"/>
     </row>
-    <row r="34" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:65">
       <c r="A34" s="6" t="s">
         <v>154</v>
       </c>
@@ -11254,7 +11254,7 @@
       <c r="BL34" s="9"/>
       <c r="BM34" s="9"/>
     </row>
-    <row r="35" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:65">
       <c r="A35" s="6" t="s">
         <v>98</v>
       </c>
@@ -11397,7 +11397,7 @@
       <c r="BL35" s="9"/>
       <c r="BM35" s="9"/>
     </row>
-    <row r="36" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:65">
       <c r="A36" s="6" t="s">
         <v>100</v>
       </c>
@@ -11526,7 +11526,7 @@
       <c r="BL36" s="9"/>
       <c r="BM36" s="9"/>
     </row>
-    <row r="37" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:65">
       <c r="A37" s="6" t="s">
         <v>102</v>
       </c>
@@ -11663,7 +11663,7 @@
       <c r="BL37" s="9"/>
       <c r="BM37" s="9"/>
     </row>
-    <row r="38" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:65">
       <c r="A38" s="6" t="s">
         <v>65</v>
       </c>
@@ -11814,7 +11814,7 @@
       <c r="BL38" s="9"/>
       <c r="BM38" s="9"/>
     </row>
-    <row r="39" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:65">
       <c r="A39" s="6" t="s">
         <v>67</v>
       </c>
@@ -11893,7 +11893,7 @@
       <c r="BL39" s="9"/>
       <c r="BM39" s="9"/>
     </row>
-    <row r="40" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:65">
       <c r="A40" s="6" t="s">
         <v>69</v>
       </c>
@@ -11980,7 +11980,7 @@
       <c r="BL40" s="9"/>
       <c r="BM40" s="9"/>
     </row>
-    <row r="41" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:65">
       <c r="A41" s="6" t="s">
         <v>136</v>
       </c>
@@ -12103,7 +12103,7 @@
       <c r="BL41" s="9"/>
       <c r="BM41" s="9"/>
     </row>
-    <row r="42" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:65">
       <c r="A42" s="6" t="s">
         <v>71</v>
       </c>
@@ -12180,7 +12180,7 @@
       <c r="BL42" s="9"/>
       <c r="BM42" s="9"/>
     </row>
-    <row r="43" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:65">
       <c r="A43" s="6" t="s">
         <v>138</v>
       </c>
@@ -12291,7 +12291,7 @@
       <c r="BL43" s="9"/>
       <c r="BM43" s="9"/>
     </row>
-    <row r="44" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:65">
       <c r="A44" s="6" t="s">
         <v>139</v>
       </c>
@@ -12404,7 +12404,7 @@
       <c r="BL44" s="9"/>
       <c r="BM44" s="9"/>
     </row>
-    <row r="45" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:65">
       <c r="A45" s="6" t="s">
         <v>103</v>
       </c>
@@ -12529,7 +12529,7 @@
       <c r="BL45" s="9"/>
       <c r="BM45" s="9"/>
     </row>
-    <row r="46" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:65">
       <c r="A46" s="6" t="s">
         <v>141</v>
       </c>
@@ -12628,7 +12628,7 @@
       <c r="BL46" s="9"/>
       <c r="BM46" s="9"/>
     </row>
-    <row r="47" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:65">
       <c r="A47" s="6" t="s">
         <v>143</v>
       </c>
@@ -12719,7 +12719,7 @@
       <c r="BL47" s="9"/>
       <c r="BM47" s="9"/>
     </row>
-    <row r="48" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:65">
       <c r="A48" s="6" t="s">
         <v>73</v>
       </c>
@@ -12876,7 +12876,7 @@
       <c r="BL48" s="9"/>
       <c r="BM48" s="9"/>
     </row>
-    <row r="49" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:65">
       <c r="A49" s="6" t="s">
         <v>65</v>
       </c>
@@ -13033,7 +13033,7 @@
       <c r="BL49" s="9"/>
       <c r="BM49" s="9"/>
     </row>
-    <row r="50" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:65">
       <c r="A50" s="6" t="s">
         <v>144</v>
       </c>
@@ -13146,7 +13146,7 @@
       <c r="BL50" s="9"/>
       <c r="BM50" s="9"/>
     </row>
-    <row r="51" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:65">
       <c r="A51" s="1" t="s">
         <v>18</v>
       </c>
@@ -13215,7 +13215,7 @@
       <c r="BL51" s="40"/>
       <c r="BM51" s="40"/>
     </row>
-    <row r="52" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:65">
       <c r="A52" s="6" t="s">
         <v>19</v>
       </c>
@@ -13310,7 +13310,7 @@
       <c r="BL52" s="9"/>
       <c r="BM52" s="9"/>
     </row>
-    <row r="53" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:65">
       <c r="A53" s="6" t="s">
         <v>22</v>
       </c>
@@ -13401,7 +13401,7 @@
       <c r="BL53" s="9"/>
       <c r="BM53" s="9"/>
     </row>
-    <row r="54" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:65">
       <c r="A54" s="6" t="s">
         <v>11</v>
       </c>
@@ -13480,7 +13480,7 @@
       <c r="BL54" s="9"/>
       <c r="BM54" s="9"/>
     </row>
-    <row r="56" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:65">
       <c r="R56" s="22" t="s">
         <v>36</v>
       </c>
@@ -13497,7 +13497,7 @@
       <c r="BB56" s="6"/>
       <c r="BJ56" s="6"/>
     </row>
-    <row r="57" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:65">
       <c r="S57" s="6" t="s">
         <v>175</v>
       </c>
@@ -13507,7 +13507,7 @@
       <c r="BB57" s="6"/>
       <c r="BJ57" s="6"/>
     </row>
-    <row r="59" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:65">
       <c r="U59" s="19" t="s">
         <v>28</v>
       </c>
@@ -13521,7 +13521,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="60" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:65">
       <c r="Y60" s="19" t="s">
         <v>28</v>
       </c>
@@ -13529,7 +13529,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="61" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:65">
       <c r="BA61" s="19" t="s">
         <v>28</v>
       </c>
@@ -13537,7 +13537,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="62" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:65">
       <c r="AF62" s="19" t="s">
         <v>28</v>
       </c>
@@ -13567,36 +13567,36 @@
       <pane xSplit="4" ySplit="8" topLeftCell="E9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="AB12" sqref="AB12"/>
+      <selection pane="bottomRight" activeCell="BM7" sqref="BM7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.5703125" customWidth="1"/>
+    <col min="6" max="6" width="3.5" customWidth="1"/>
     <col min="7" max="14" width="3" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="3" customWidth="1"/>
     <col min="16" max="21" width="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="2.7109375" customWidth="1"/>
+    <col min="22" max="22" width="2.6640625" customWidth="1"/>
     <col min="23" max="26" width="3" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="3.42578125" customWidth="1"/>
+    <col min="27" max="27" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="3.5" customWidth="1"/>
     <col min="29" max="37" width="3" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="3.7109375" customWidth="1"/>
+    <col min="38" max="38" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="3.6640625" customWidth="1"/>
     <col min="40" max="45" width="3" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="3.140625" customWidth="1"/>
+    <col min="46" max="46" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="3.1640625" customWidth="1"/>
     <col min="48" max="56" width="3" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="3.28515625" customWidth="1"/>
+    <col min="57" max="57" width="3.33203125" customWidth="1"/>
     <col min="58" max="65" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:65">
       <c r="A1" s="41" t="s">
         <v>25</v>
       </c>
@@ -13665,7 +13665,7 @@
       <c r="BL1" s="6"/>
       <c r="BM1" s="6"/>
     </row>
-    <row r="2" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:65">
       <c r="A2" s="41"/>
       <c r="B2" s="41"/>
       <c r="C2" s="41"/>
@@ -13758,7 +13758,7 @@
       <c r="BL2" s="6"/>
       <c r="BM2" s="6"/>
     </row>
-    <row r="3" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:65">
       <c r="A3" s="41"/>
       <c r="B3" s="41"/>
       <c r="C3" s="41"/>
@@ -13851,7 +13851,7 @@
       <c r="BL3" s="6"/>
       <c r="BM3" s="6"/>
     </row>
-    <row r="4" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:65">
       <c r="A4" s="23"/>
       <c r="B4" s="23"/>
       <c r="C4" s="23"/>
@@ -13930,7 +13930,7 @@
       <c r="BL4" s="6"/>
       <c r="BM4" s="6"/>
     </row>
-    <row r="6" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:65">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -14003,7 +14003,7 @@
       <c r="BL6" s="43"/>
       <c r="BM6" s="43"/>
     </row>
-    <row r="7" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:65">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -14017,190 +14017,190 @@
         <v>4</v>
       </c>
       <c r="E7" s="24">
-        <v>44440</v>
+        <v>45047</v>
       </c>
       <c r="F7" s="24">
-        <v>44441</v>
+        <v>45048</v>
       </c>
       <c r="G7" s="24">
-        <v>44442</v>
+        <v>45049</v>
       </c>
       <c r="H7" s="24">
-        <v>44443</v>
+        <v>45050</v>
       </c>
       <c r="I7" s="24">
-        <v>44444</v>
+        <v>45051</v>
       </c>
       <c r="J7" s="24">
-        <v>44445</v>
+        <v>45052</v>
       </c>
       <c r="K7" s="24">
-        <v>44446</v>
+        <v>45053</v>
       </c>
       <c r="L7" s="24">
-        <v>44447</v>
+        <v>45054</v>
       </c>
       <c r="M7" s="24">
-        <v>44448</v>
+        <v>45055</v>
       </c>
       <c r="N7" s="24">
-        <v>44449</v>
+        <v>45056</v>
       </c>
       <c r="O7" s="24">
-        <v>44450</v>
+        <v>45057</v>
       </c>
       <c r="P7" s="24">
-        <v>44451</v>
+        <v>45058</v>
       </c>
       <c r="Q7" s="24">
-        <v>44452</v>
+        <v>45059</v>
       </c>
       <c r="R7" s="24">
-        <v>44453</v>
+        <v>45060</v>
       </c>
       <c r="S7" s="24">
-        <v>44454</v>
+        <v>45061</v>
       </c>
       <c r="T7" s="24">
-        <v>44455</v>
+        <v>45062</v>
       </c>
       <c r="U7" s="24">
-        <v>44456</v>
+        <v>45063</v>
       </c>
       <c r="V7" s="24">
-        <v>44457</v>
+        <v>45064</v>
       </c>
       <c r="W7" s="24">
-        <v>44458</v>
+        <v>45065</v>
       </c>
       <c r="X7" s="24">
-        <v>44459</v>
+        <v>45066</v>
       </c>
       <c r="Y7" s="24">
-        <v>44460</v>
+        <v>45067</v>
       </c>
       <c r="Z7" s="24">
-        <v>44461</v>
+        <v>45068</v>
       </c>
       <c r="AA7" s="24">
-        <v>44462</v>
+        <v>45069</v>
       </c>
       <c r="AB7" s="24">
-        <v>44463</v>
+        <v>45070</v>
       </c>
       <c r="AC7" s="24">
-        <v>44464</v>
+        <v>45071</v>
       </c>
       <c r="AD7" s="24">
-        <v>44465</v>
+        <v>45072</v>
       </c>
       <c r="AE7" s="24">
-        <v>44466</v>
+        <v>45073</v>
       </c>
       <c r="AF7" s="24">
-        <v>44467</v>
+        <v>45074</v>
       </c>
       <c r="AG7" s="24">
-        <v>44468</v>
+        <v>45075</v>
       </c>
       <c r="AH7" s="24">
-        <v>44469</v>
+        <v>45076</v>
       </c>
       <c r="AI7" s="24">
-        <v>31</v>
+        <v>45077</v>
       </c>
       <c r="AJ7" s="24">
-        <v>44470</v>
+        <v>45078</v>
       </c>
       <c r="AK7" s="24">
-        <v>44471</v>
+        <v>45079</v>
       </c>
       <c r="AL7" s="24">
-        <v>44472</v>
+        <v>45080</v>
       </c>
       <c r="AM7" s="24">
-        <v>44473</v>
+        <v>45081</v>
       </c>
       <c r="AN7" s="24">
-        <v>44474</v>
+        <v>45082</v>
       </c>
       <c r="AO7" s="24">
-        <v>44475</v>
+        <v>45083</v>
       </c>
       <c r="AP7" s="24">
-        <v>44476</v>
+        <v>45084</v>
       </c>
       <c r="AQ7" s="24">
-        <v>44477</v>
+        <v>45085</v>
       </c>
       <c r="AR7" s="24">
-        <v>44478</v>
+        <v>45086</v>
       </c>
       <c r="AS7" s="24">
-        <v>44479</v>
+        <v>45087</v>
       </c>
       <c r="AT7" s="24">
-        <v>44480</v>
+        <v>45088</v>
       </c>
       <c r="AU7" s="24">
-        <v>44481</v>
+        <v>45089</v>
       </c>
       <c r="AV7" s="24">
-        <v>44482</v>
+        <v>45090</v>
       </c>
       <c r="AW7" s="24">
-        <v>44483</v>
+        <v>45091</v>
       </c>
       <c r="AX7" s="24">
-        <v>44484</v>
+        <v>45092</v>
       </c>
       <c r="AY7" s="24">
-        <v>44485</v>
+        <v>45093</v>
       </c>
       <c r="AZ7" s="24">
-        <v>44486</v>
+        <v>45094</v>
       </c>
       <c r="BA7" s="24">
-        <v>44487</v>
+        <v>45095</v>
       </c>
       <c r="BB7" s="24">
-        <v>44488</v>
+        <v>45096</v>
       </c>
       <c r="BC7" s="24">
-        <v>44489</v>
+        <v>45097</v>
       </c>
       <c r="BD7" s="24">
-        <v>44490</v>
+        <v>45098</v>
       </c>
       <c r="BE7" s="24">
-        <v>44491</v>
+        <v>45099</v>
       </c>
       <c r="BF7" s="24">
-        <v>44492</v>
+        <v>45100</v>
       </c>
       <c r="BG7" s="24">
-        <v>44493</v>
+        <v>45101</v>
       </c>
       <c r="BH7" s="24">
-        <v>44494</v>
+        <v>45102</v>
       </c>
       <c r="BI7" s="24">
-        <v>44495</v>
+        <v>45103</v>
       </c>
       <c r="BJ7" s="24">
-        <v>44496</v>
+        <v>45104</v>
       </c>
       <c r="BK7" s="24">
-        <v>28</v>
+        <v>45105</v>
       </c>
       <c r="BL7" s="24">
-        <v>29</v>
+        <v>45106</v>
       </c>
       <c r="BM7" s="24">
-        <v>30</v>
+        <v>45107</v>
       </c>
     </row>
-    <row r="8" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:65">
       <c r="A8" s="44" t="s">
         <v>5</v>
       </c>
@@ -14277,7 +14277,7 @@
       <c r="BL8" s="26"/>
       <c r="BM8" s="26"/>
     </row>
-    <row r="9" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:65">
       <c r="A9" s="5" t="s">
         <v>113</v>
       </c>
@@ -14374,7 +14374,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:65">
       <c r="A10" s="5" t="s">
         <v>115</v>
       </c>
@@ -14485,7 +14485,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:65">
       <c r="A11" s="5" t="s">
         <v>117</v>
       </c>
@@ -14586,7 +14586,7 @@
       <c r="BL11" s="26"/>
       <c r="BM11" s="26"/>
     </row>
-    <row r="12" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:65">
       <c r="A12" s="5" t="s">
         <v>119</v>
       </c>
@@ -14689,7 +14689,7 @@
       <c r="BL12" s="26"/>
       <c r="BM12" s="26"/>
     </row>
-    <row r="13" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:65">
       <c r="A13" s="5" t="s">
         <v>121</v>
       </c>
@@ -14790,7 +14790,7 @@
       <c r="BL13" s="26"/>
       <c r="BM13" s="26"/>
     </row>
-    <row r="14" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:65">
       <c r="A14" s="5" t="s">
         <v>94</v>
       </c>
@@ -14893,7 +14893,7 @@
       <c r="BL14" s="26"/>
       <c r="BM14" s="26"/>
     </row>
-    <row r="15" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:65">
       <c r="A15" s="5" t="s">
         <v>96</v>
       </c>
@@ -14992,7 +14992,7 @@
       <c r="BL15" s="26"/>
       <c r="BM15" s="26"/>
     </row>
-    <row r="16" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:65">
       <c r="A16" s="5" t="s">
         <v>90</v>
       </c>
@@ -15101,7 +15101,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:65">
       <c r="A17" s="5" t="s">
         <v>92</v>
       </c>
@@ -15208,7 +15208,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:65">
       <c r="A18" s="5" t="s">
         <v>53</v>
       </c>
@@ -15315,7 +15315,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:65">
       <c r="A19" s="5" t="s">
         <v>180</v>
       </c>
@@ -15414,7 +15414,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:65">
       <c r="A20" s="5" t="s">
         <v>57</v>
       </c>
@@ -15521,7 +15521,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:65">
       <c r="A21" s="5" t="s">
         <v>55</v>
       </c>
@@ -15626,7 +15626,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:65">
       <c r="A22" s="5" t="s">
         <v>123</v>
       </c>
@@ -15745,7 +15745,7 @@
       <c r="BL22" s="26"/>
       <c r="BM22" s="26"/>
     </row>
-    <row r="23" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:65">
       <c r="A23" s="5" t="s">
         <v>124</v>
       </c>
@@ -15864,7 +15864,7 @@
       <c r="BL23" s="26"/>
       <c r="BM23" s="26"/>
     </row>
-    <row r="24" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:65">
       <c r="A24" s="5" t="s">
         <v>125</v>
       </c>
@@ -15971,7 +15971,7 @@
       <c r="BL24" s="26"/>
       <c r="BM24" s="26"/>
     </row>
-    <row r="25" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:65">
       <c r="A25" s="5" t="s">
         <v>127</v>
       </c>
@@ -16092,7 +16092,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:65">
       <c r="A26" s="5" t="s">
         <v>88</v>
       </c>
@@ -16185,7 +16185,7 @@
       <c r="BL26" s="18"/>
       <c r="BM26" s="18"/>
     </row>
-    <row r="27" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:65">
       <c r="A27" s="5" t="s">
         <v>130</v>
       </c>
@@ -16294,7 +16294,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:65">
       <c r="A28" s="5" t="s">
         <v>63</v>
       </c>
@@ -16387,7 +16387,7 @@
       <c r="BL28" s="26"/>
       <c r="BM28" s="26"/>
     </row>
-    <row r="29" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:65">
       <c r="A29" s="5" t="s">
         <v>134</v>
       </c>
@@ -16488,7 +16488,7 @@
       </c>
       <c r="BM29" s="26"/>
     </row>
-    <row r="30" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:65">
       <c r="A30" s="5" t="s">
         <v>89</v>
       </c>
@@ -16593,7 +16593,7 @@
       <c r="BL30" s="26"/>
       <c r="BM30" s="26"/>
     </row>
-    <row r="31" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:65">
       <c r="A31" s="1" t="s">
         <v>13</v>
       </c>
@@ -16662,7 +16662,7 @@
       <c r="BL31" s="40"/>
       <c r="BM31" s="40"/>
     </row>
-    <row r="32" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:65">
       <c r="A32" s="6" t="s">
         <v>146</v>
       </c>
@@ -16819,7 +16819,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:65">
       <c r="A33" s="6" t="s">
         <v>154</v>
       </c>
@@ -16976,7 +16976,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:65">
       <c r="A34" s="6" t="s">
         <v>98</v>
       </c>
@@ -17055,7 +17055,7 @@
       <c r="BL34" s="26"/>
       <c r="BM34" s="26"/>
     </row>
-    <row r="35" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:65">
       <c r="A35" s="6" t="s">
         <v>100</v>
       </c>
@@ -17220,7 +17220,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:65">
       <c r="A36" s="6" t="s">
         <v>102</v>
       </c>
@@ -17385,7 +17385,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:65">
       <c r="A37" s="6" t="s">
         <v>65</v>
       </c>
@@ -17496,7 +17496,7 @@
       <c r="BL37" s="26"/>
       <c r="BM37" s="26"/>
     </row>
-    <row r="38" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:65">
       <c r="A38" s="6" t="s">
         <v>67</v>
       </c>
@@ -17645,7 +17645,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:65">
       <c r="A39" s="6" t="s">
         <v>69</v>
       </c>
@@ -17794,7 +17794,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:65">
       <c r="A40" s="6" t="s">
         <v>136</v>
       </c>
@@ -17951,7 +17951,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:65">
       <c r="A41" s="6" t="s">
         <v>71</v>
       </c>
@@ -18092,7 +18092,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:65">
       <c r="A42" s="6" t="s">
         <v>138</v>
       </c>
@@ -18249,7 +18249,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:65">
       <c r="A43" s="6" t="s">
         <v>139</v>
       </c>
@@ -18406,7 +18406,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:65">
       <c r="A44" s="6" t="s">
         <v>103</v>
       </c>
@@ -18501,7 +18501,7 @@
       <c r="BL44" s="26"/>
       <c r="BM44" s="26"/>
     </row>
-    <row r="45" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:65">
       <c r="A45" s="6" t="s">
         <v>141</v>
       </c>
@@ -18650,7 +18650,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:65">
       <c r="A46" s="6" t="s">
         <v>143</v>
       </c>
@@ -18801,7 +18801,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:65">
       <c r="A47" s="6" t="s">
         <v>73</v>
       </c>
@@ -18884,7 +18884,7 @@
       <c r="BL47" s="26"/>
       <c r="BM47" s="26"/>
     </row>
-    <row r="48" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:65">
       <c r="A48" s="6" t="s">
         <v>65</v>
       </c>
@@ -18967,7 +18967,7 @@
       <c r="BL48" s="26"/>
       <c r="BM48" s="26"/>
     </row>
-    <row r="49" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:65">
       <c r="A49" s="1" t="s">
         <v>18</v>
       </c>
@@ -19036,7 +19036,7 @@
       <c r="BL49" s="40"/>
       <c r="BM49" s="40"/>
     </row>
-    <row r="50" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:65">
       <c r="A50" s="6" t="s">
         <v>19</v>
       </c>
@@ -19125,7 +19125,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:65">
       <c r="A51" s="6" t="s">
         <v>22</v>
       </c>
@@ -19210,7 +19210,7 @@
       <c r="BL51" s="26"/>
       <c r="BM51" s="26"/>
     </row>
-    <row r="52" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:65">
       <c r="A52" s="6" t="s">
         <v>11</v>
       </c>
@@ -19313,7 +19313,7 @@
       <c r="BL52" s="26"/>
       <c r="BM52" s="26"/>
     </row>
-    <row r="54" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:65">
       <c r="F54" s="22" t="s">
         <v>36</v>
       </c>
@@ -19327,7 +19327,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="55" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:65">
       <c r="G55" s="6" t="s">
         <v>178</v>
       </c>
@@ -19335,7 +19335,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="56" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:65">
       <c r="BD56" s="19" t="s">
         <v>28</v>
       </c>
@@ -19370,35 +19370,35 @@
       <selection pane="bottomRight" activeCell="BK34" sqref="BK34:BN34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.85546875" customWidth="1"/>
+    <col min="6" max="6" width="2.83203125" customWidth="1"/>
     <col min="7" max="13" width="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="3.28515625" customWidth="1"/>
-    <col min="15" max="15" width="2.85546875" customWidth="1"/>
+    <col min="14" max="14" width="3.33203125" customWidth="1"/>
+    <col min="15" max="15" width="2.83203125" customWidth="1"/>
     <col min="16" max="21" width="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="2.7109375" customWidth="1"/>
+    <col min="22" max="22" width="2.6640625" customWidth="1"/>
     <col min="23" max="26" width="3" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="3.28515625" customWidth="1"/>
+    <col min="27" max="27" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="3.33203125" customWidth="1"/>
     <col min="29" max="37" width="3" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="3.42578125" customWidth="1"/>
+    <col min="38" max="38" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="3.5" customWidth="1"/>
     <col min="40" max="45" width="3" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="3.42578125" customWidth="1"/>
+    <col min="46" max="46" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="3.5" customWidth="1"/>
     <col min="48" max="56" width="3" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="2.7109375" customWidth="1"/>
+    <col min="57" max="57" width="2.6640625" customWidth="1"/>
     <col min="58" max="65" width="3" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:66">
       <c r="A1" s="41" t="s">
         <v>25</v>
       </c>
@@ -19468,7 +19468,7 @@
       <c r="BM1" s="6"/>
       <c r="BN1" s="6"/>
     </row>
-    <row r="2" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:66">
       <c r="A2" s="41"/>
       <c r="B2" s="41"/>
       <c r="C2" s="41"/>
@@ -19562,7 +19562,7 @@
       <c r="BM2" s="6"/>
       <c r="BN2" s="6"/>
     </row>
-    <row r="3" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:66">
       <c r="A3" s="41"/>
       <c r="B3" s="41"/>
       <c r="C3" s="41"/>
@@ -19656,7 +19656,7 @@
       <c r="BM3" s="6"/>
       <c r="BN3" s="6"/>
     </row>
-    <row r="4" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:66">
       <c r="A4" s="23"/>
       <c r="B4" s="23"/>
       <c r="C4" s="23"/>
@@ -19736,7 +19736,7 @@
       <c r="BM4" s="6"/>
       <c r="BN4" s="6"/>
     </row>
-    <row r="6" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:66">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -19810,7 +19810,7 @@
       <c r="BM6" s="43"/>
       <c r="BN6" s="52"/>
     </row>
-    <row r="7" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:66">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -20010,7 +20010,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:66">
       <c r="A8" s="44" t="s">
         <v>5</v>
       </c>
@@ -20080,7 +20080,7 @@
       <c r="BM8" s="18"/>
       <c r="BN8" s="18"/>
     </row>
-    <row r="9" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:66">
       <c r="A9" s="5" t="s">
         <v>113</v>
       </c>
@@ -20164,7 +20164,7 @@
       <c r="BM9" s="18"/>
       <c r="BN9" s="18"/>
     </row>
-    <row r="10" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:66">
       <c r="A10" s="5" t="s">
         <v>115</v>
       </c>
@@ -20248,7 +20248,7 @@
       <c r="BM10" s="18"/>
       <c r="BN10" s="18"/>
     </row>
-    <row r="11" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:66">
       <c r="A11" s="5" t="s">
         <v>117</v>
       </c>
@@ -20336,7 +20336,7 @@
       <c r="BM11" s="18"/>
       <c r="BN11" s="18"/>
     </row>
-    <row r="12" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:66">
       <c r="A12" s="5" t="s">
         <v>119</v>
       </c>
@@ -20424,7 +20424,7 @@
       <c r="BM12" s="18"/>
       <c r="BN12" s="18"/>
     </row>
-    <row r="13" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:66">
       <c r="A13" s="5" t="s">
         <v>121</v>
       </c>
@@ -20532,7 +20532,7 @@
       <c r="BM13" s="18"/>
       <c r="BN13" s="18"/>
     </row>
-    <row r="14" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:66">
       <c r="A14" s="5" t="s">
         <v>94</v>
       </c>
@@ -20650,7 +20650,7 @@
       <c r="BM14" s="18"/>
       <c r="BN14" s="18"/>
     </row>
-    <row r="15" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:66">
       <c r="A15" s="5" t="s">
         <v>96</v>
       </c>
@@ -20738,7 +20738,7 @@
       <c r="BM15" s="18"/>
       <c r="BN15" s="18"/>
     </row>
-    <row r="16" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:66">
       <c r="A16" s="5" t="s">
         <v>90</v>
       </c>
@@ -20822,7 +20822,7 @@
       <c r="BM16" s="18"/>
       <c r="BN16" s="18"/>
     </row>
-    <row r="17" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:66">
       <c r="A17" s="5" t="s">
         <v>92</v>
       </c>
@@ -20936,7 +20936,7 @@
       <c r="BM17" s="18"/>
       <c r="BN17" s="18"/>
     </row>
-    <row r="18" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:66">
       <c r="A18" s="5" t="s">
         <v>53</v>
       </c>
@@ -21038,7 +21038,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:66">
       <c r="A19" s="5" t="s">
         <v>180</v>
       </c>
@@ -21150,7 +21150,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:66">
       <c r="A20" s="5" t="s">
         <v>57</v>
       </c>
@@ -21234,7 +21234,7 @@
       <c r="BM20" s="18"/>
       <c r="BN20" s="18"/>
     </row>
-    <row r="21" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:66">
       <c r="A21" s="5" t="s">
         <v>55</v>
       </c>
@@ -21372,7 +21372,7 @@
       <c r="BM21" s="18"/>
       <c r="BN21" s="18"/>
     </row>
-    <row r="22" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:66">
       <c r="A22" s="5" t="s">
         <v>123</v>
       </c>
@@ -21464,7 +21464,7 @@
       <c r="BM22" s="18"/>
       <c r="BN22" s="18"/>
     </row>
-    <row r="23" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:66">
       <c r="A23" s="5" t="s">
         <v>124</v>
       </c>
@@ -21556,7 +21556,7 @@
       <c r="BM23" s="18"/>
       <c r="BN23" s="18"/>
     </row>
-    <row r="24" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:66">
       <c r="A24" s="5" t="s">
         <v>125</v>
       </c>
@@ -21694,7 +21694,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:66">
       <c r="A25" s="5" t="s">
         <v>127</v>
       </c>
@@ -21806,7 +21806,7 @@
       <c r="BM25" s="18"/>
       <c r="BN25" s="18"/>
     </row>
-    <row r="26" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:66">
       <c r="A26" s="5" t="s">
         <v>88</v>
       </c>
@@ -21882,7 +21882,7 @@
       <c r="BM26" s="26"/>
       <c r="BN26" s="26"/>
     </row>
-    <row r="27" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:66">
       <c r="A27" s="5" t="s">
         <v>130</v>
       </c>
@@ -21992,7 +21992,7 @@
       <c r="BM27" s="18"/>
       <c r="BN27" s="18"/>
     </row>
-    <row r="28" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:66">
       <c r="A28" s="5" t="s">
         <v>63</v>
       </c>
@@ -22068,7 +22068,7 @@
       <c r="BM28" s="18"/>
       <c r="BN28" s="18"/>
     </row>
-    <row r="29" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:66">
       <c r="A29" s="5" t="s">
         <v>134</v>
       </c>
@@ -22174,7 +22174,7 @@
       <c r="BM29" s="18"/>
       <c r="BN29" s="18"/>
     </row>
-    <row r="30" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:66">
       <c r="A30" s="5" t="s">
         <v>89</v>
       </c>
@@ -22270,7 +22270,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:66">
       <c r="A31" s="1" t="s">
         <v>13</v>
       </c>
@@ -22340,7 +22340,7 @@
       <c r="BM31" s="40"/>
       <c r="BN31" s="34"/>
     </row>
-    <row r="32" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:66">
       <c r="A32" s="6" t="s">
         <v>146</v>
       </c>
@@ -22436,7 +22436,7 @@
       <c r="BM32" s="30"/>
       <c r="BN32" s="26"/>
     </row>
-    <row r="33" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:66">
       <c r="A33" s="6" t="s">
         <v>154</v>
       </c>
@@ -22532,7 +22532,7 @@
       <c r="BM33" s="30"/>
       <c r="BN33" s="26"/>
     </row>
-    <row r="34" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:66">
       <c r="A34" s="6" t="s">
         <v>98</v>
       </c>
@@ -22616,7 +22616,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:66">
       <c r="A35" s="6" t="s">
         <v>100</v>
       </c>
@@ -22758,7 +22758,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:66">
       <c r="A36" s="6" t="s">
         <v>102</v>
       </c>
@@ -22872,7 +22872,7 @@
       <c r="BM36" s="30"/>
       <c r="BN36" s="26"/>
     </row>
-    <row r="37" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:66">
       <c r="A37" s="6" t="s">
         <v>65</v>
       </c>
@@ -22948,7 +22948,7 @@
       <c r="BM37" s="30"/>
       <c r="BN37" s="26"/>
     </row>
-    <row r="38" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:66">
       <c r="A38" s="6" t="s">
         <v>67</v>
       </c>
@@ -23074,7 +23074,7 @@
       <c r="BM38" s="30"/>
       <c r="BN38" s="26"/>
     </row>
-    <row r="39" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:66">
       <c r="A39" s="6" t="s">
         <v>69</v>
       </c>
@@ -23200,7 +23200,7 @@
       <c r="BM39" s="30"/>
       <c r="BN39" s="26"/>
     </row>
-    <row r="40" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:66">
       <c r="A40" s="6" t="s">
         <v>136</v>
       </c>
@@ -23276,7 +23276,7 @@
       <c r="BM40" s="30"/>
       <c r="BN40" s="26"/>
     </row>
-    <row r="41" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:66">
       <c r="A41" s="6" t="s">
         <v>71</v>
       </c>
@@ -23432,7 +23432,7 @@
       <c r="BM41" s="30"/>
       <c r="BN41" s="26"/>
     </row>
-    <row r="42" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:66">
       <c r="A42" s="6" t="s">
         <v>138</v>
       </c>
@@ -23508,7 +23508,7 @@
       <c r="BM42" s="30"/>
       <c r="BN42" s="26"/>
     </row>
-    <row r="43" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:66">
       <c r="A43" s="6" t="s">
         <v>139</v>
       </c>
@@ -23584,7 +23584,7 @@
       <c r="BM43" s="30"/>
       <c r="BN43" s="26"/>
     </row>
-    <row r="44" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:66">
       <c r="A44" s="6" t="s">
         <v>103</v>
       </c>
@@ -23672,7 +23672,7 @@
       <c r="BM44" s="30"/>
       <c r="BN44" s="26"/>
     </row>
-    <row r="45" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:66">
       <c r="A45" s="6" t="s">
         <v>141</v>
       </c>
@@ -23808,7 +23808,7 @@
       <c r="BM45" s="30"/>
       <c r="BN45" s="26"/>
     </row>
-    <row r="46" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:66">
       <c r="A46" s="6" t="s">
         <v>143</v>
       </c>
@@ -23944,7 +23944,7 @@
       <c r="BM46" s="30"/>
       <c r="BN46" s="26"/>
     </row>
-    <row r="47" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:66">
       <c r="A47" s="6" t="s">
         <v>73</v>
       </c>
@@ -24020,7 +24020,7 @@
       <c r="BM47" s="30"/>
       <c r="BN47" s="26"/>
     </row>
-    <row r="48" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:66">
       <c r="A48" s="6" t="s">
         <v>65</v>
       </c>
@@ -24096,7 +24096,7 @@
       <c r="BM48" s="30"/>
       <c r="BN48" s="26"/>
     </row>
-    <row r="49" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:66">
       <c r="A49" s="1" t="s">
         <v>18</v>
       </c>
@@ -24166,7 +24166,7 @@
       <c r="BM49" s="40"/>
       <c r="BN49" s="34"/>
     </row>
-    <row r="50" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:66">
       <c r="A50" s="6" t="s">
         <v>19</v>
       </c>
@@ -24276,7 +24276,7 @@
       <c r="BM50" s="30"/>
       <c r="BN50" s="26"/>
     </row>
-    <row r="51" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:66">
       <c r="A51" s="6" t="s">
         <v>22</v>
       </c>
@@ -24364,7 +24364,7 @@
       <c r="BM51" s="30"/>
       <c r="BN51" s="26"/>
     </row>
-    <row r="52" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:66">
       <c r="A52" s="6" t="s">
         <v>11</v>
       </c>
@@ -24485,33 +24485,33 @@
       <selection pane="bottomRight" activeCell="H36" sqref="H36:L36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.5703125" customWidth="1"/>
+    <col min="6" max="6" width="3.5" customWidth="1"/>
     <col min="7" max="14" width="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="3.85546875" customWidth="1"/>
+    <col min="15" max="15" width="3.83203125" customWidth="1"/>
     <col min="16" max="21" width="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="3.42578125" customWidth="1"/>
+    <col min="22" max="22" width="3.5" customWidth="1"/>
     <col min="23" max="26" width="3" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="3.5703125" customWidth="1"/>
+    <col min="27" max="27" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="3.5" customWidth="1"/>
     <col min="29" max="36" width="3" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="3.85546875" customWidth="1"/>
+    <col min="37" max="37" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="3.83203125" customWidth="1"/>
     <col min="39" max="44" width="3" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="3.42578125" customWidth="1"/>
+    <col min="45" max="45" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="3.5" customWidth="1"/>
     <col min="47" max="55" width="3" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="3.28515625" customWidth="1"/>
+    <col min="56" max="56" width="3.33203125" customWidth="1"/>
     <col min="57" max="65" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:65">
       <c r="A1" s="41" t="s">
         <v>25</v>
       </c>
@@ -24580,7 +24580,7 @@
       <c r="BL1" s="6"/>
       <c r="BM1" s="6"/>
     </row>
-    <row r="2" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:65">
       <c r="A2" s="41"/>
       <c r="B2" s="41"/>
       <c r="C2" s="41"/>
@@ -24673,7 +24673,7 @@
       <c r="BL2" s="6"/>
       <c r="BM2" s="6"/>
     </row>
-    <row r="3" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:65">
       <c r="A3" s="41"/>
       <c r="B3" s="41"/>
       <c r="C3" s="41"/>
@@ -24766,7 +24766,7 @@
       <c r="BL3" s="6"/>
       <c r="BM3" s="6"/>
     </row>
-    <row r="4" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:65">
       <c r="A4" s="23"/>
       <c r="B4" s="23"/>
       <c r="C4" s="23"/>
@@ -24845,7 +24845,7 @@
       <c r="BL4" s="6"/>
       <c r="BM4" s="6"/>
     </row>
-    <row r="6" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:65">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -24918,7 +24918,7 @@
       <c r="BL6" s="43"/>
       <c r="BM6" s="52"/>
     </row>
-    <row r="7" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:65">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -25115,7 +25115,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:65">
       <c r="A8" s="44" t="s">
         <v>5</v>
       </c>
@@ -25184,7 +25184,7 @@
       <c r="BL8" s="18"/>
       <c r="BM8" s="18"/>
     </row>
-    <row r="9" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:65">
       <c r="A9" s="5" t="s">
         <v>113</v>
       </c>
@@ -25269,7 +25269,7 @@
       <c r="BL9" s="18"/>
       <c r="BM9" s="18"/>
     </row>
-    <row r="10" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:65">
       <c r="A10" s="5" t="s">
         <v>115</v>
       </c>
@@ -25354,7 +25354,7 @@
       <c r="BL10" s="18"/>
       <c r="BM10" s="18"/>
     </row>
-    <row r="11" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:65">
       <c r="A11" s="5" t="s">
         <v>117</v>
       </c>
@@ -25441,7 +25441,7 @@
       <c r="BL11" s="18"/>
       <c r="BM11" s="18"/>
     </row>
-    <row r="12" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:65">
       <c r="A12" s="5" t="s">
         <v>119</v>
       </c>
@@ -25526,7 +25526,7 @@
       <c r="BL12" s="18"/>
       <c r="BM12" s="18"/>
     </row>
-    <row r="13" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:65">
       <c r="A13" s="5" t="s">
         <v>121</v>
       </c>
@@ -25611,7 +25611,7 @@
       <c r="BL13" s="18"/>
       <c r="BM13" s="18"/>
     </row>
-    <row r="14" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:65">
       <c r="A14" s="5" t="s">
         <v>94</v>
       </c>
@@ -25686,7 +25686,7 @@
       <c r="BL14" s="18"/>
       <c r="BM14" s="18"/>
     </row>
-    <row r="15" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:65">
       <c r="A15" s="5" t="s">
         <v>96</v>
       </c>
@@ -25765,7 +25765,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:65">
       <c r="A16" s="5" t="s">
         <v>90</v>
       </c>
@@ -25840,7 +25840,7 @@
       <c r="BL16" s="18"/>
       <c r="BM16" s="18"/>
     </row>
-    <row r="17" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:65">
       <c r="A17" s="5" t="s">
         <v>92</v>
       </c>
@@ -25915,7 +25915,7 @@
       <c r="BL17" s="18"/>
       <c r="BM17" s="18"/>
     </row>
-    <row r="18" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:65">
       <c r="A18" s="5" t="s">
         <v>53</v>
       </c>
@@ -26006,7 +26006,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:65">
       <c r="A19" s="5" t="s">
         <v>180</v>
       </c>
@@ -26083,7 +26083,7 @@
       <c r="BL19" s="18"/>
       <c r="BM19" s="18"/>
     </row>
-    <row r="20" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:65">
       <c r="A20" s="5" t="s">
         <v>57</v>
       </c>
@@ -26158,7 +26158,7 @@
       <c r="BL20" s="18"/>
       <c r="BM20" s="18"/>
     </row>
-    <row r="21" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:65">
       <c r="A21" s="5" t="s">
         <v>55</v>
       </c>
@@ -26233,7 +26233,7 @@
       <c r="BL21" s="18"/>
       <c r="BM21" s="18"/>
     </row>
-    <row r="22" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:65">
       <c r="A22" s="5" t="s">
         <v>123</v>
       </c>
@@ -26322,7 +26322,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:65">
       <c r="A23" s="5" t="s">
         <v>124</v>
       </c>
@@ -26407,7 +26407,7 @@
       <c r="BL23" s="18"/>
       <c r="BM23" s="18"/>
     </row>
-    <row r="24" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:65">
       <c r="A24" s="5" t="s">
         <v>125</v>
       </c>
@@ -26492,7 +26492,7 @@
       <c r="BL24" s="18"/>
       <c r="BM24" s="18"/>
     </row>
-    <row r="25" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:65">
       <c r="A25" s="5" t="s">
         <v>127</v>
       </c>
@@ -26577,7 +26577,7 @@
       <c r="BL25" s="18"/>
       <c r="BM25" s="18"/>
     </row>
-    <row r="26" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:65">
       <c r="A26" s="5" t="s">
         <v>88</v>
       </c>
@@ -26652,7 +26652,7 @@
       <c r="BL26" s="18"/>
       <c r="BM26" s="18"/>
     </row>
-    <row r="27" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:65">
       <c r="A27" s="5" t="s">
         <v>59</v>
       </c>
@@ -26727,7 +26727,7 @@
       <c r="BL27" s="18"/>
       <c r="BM27" s="18"/>
     </row>
-    <row r="28" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:65">
       <c r="A28" s="5" t="s">
         <v>61</v>
       </c>
@@ -26802,7 +26802,7 @@
       <c r="BL28" s="18"/>
       <c r="BM28" s="18"/>
     </row>
-    <row r="29" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:65">
       <c r="A29" s="5" t="s">
         <v>130</v>
       </c>
@@ -26893,7 +26893,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:65">
       <c r="A30" s="5" t="s">
         <v>63</v>
       </c>
@@ -26968,7 +26968,7 @@
       <c r="BL30" s="18"/>
       <c r="BM30" s="18"/>
     </row>
-    <row r="31" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:65">
       <c r="A31" s="5" t="s">
         <v>134</v>
       </c>
@@ -27057,7 +27057,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:65">
       <c r="A32" s="5" t="s">
         <v>89</v>
       </c>
@@ -27138,7 +27138,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:65">
       <c r="A33" s="1" t="s">
         <v>13</v>
       </c>
@@ -27207,7 +27207,7 @@
       <c r="BL33" s="53"/>
       <c r="BM33" s="34"/>
     </row>
-    <row r="34" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:65">
       <c r="A34" s="6" t="s">
         <v>146</v>
       </c>
@@ -27334,7 +27334,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:65">
       <c r="A35" s="6" t="s">
         <v>154</v>
       </c>
@@ -27461,7 +27461,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:65">
       <c r="A36" s="6" t="s">
         <v>98</v>
       </c>
@@ -27620,7 +27620,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:65">
       <c r="A37" s="6" t="s">
         <v>100</v>
       </c>
@@ -27779,7 +27779,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:65">
       <c r="A38" s="6" t="s">
         <v>102</v>
       </c>
@@ -27926,7 +27926,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:65">
       <c r="A39" s="6" t="s">
         <v>65</v>
       </c>
@@ -28003,7 +28003,7 @@
       <c r="BL39" s="54"/>
       <c r="BM39" s="54"/>
     </row>
-    <row r="40" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:65">
       <c r="A40" s="6" t="s">
         <v>67</v>
       </c>
@@ -28080,7 +28080,7 @@
       <c r="BL40" s="54"/>
       <c r="BM40" s="54"/>
     </row>
-    <row r="41" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:65">
       <c r="A41" s="6" t="s">
         <v>69</v>
       </c>
@@ -28157,7 +28157,7 @@
       <c r="BL41" s="54"/>
       <c r="BM41" s="54"/>
     </row>
-    <row r="42" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:65">
       <c r="A42" s="6" t="s">
         <v>136</v>
       </c>
@@ -28314,7 +28314,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:65">
       <c r="A43" s="6" t="s">
         <v>71</v>
       </c>
@@ -28391,7 +28391,7 @@
       <c r="BL43" s="54"/>
       <c r="BM43" s="54"/>
     </row>
-    <row r="44" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:65">
       <c r="A44" s="6" t="s">
         <v>138</v>
       </c>
@@ -28548,7 +28548,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:65">
       <c r="A45" s="6" t="s">
         <v>139</v>
       </c>
@@ -28705,7 +28705,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:65">
       <c r="A46" s="6" t="s">
         <v>103</v>
       </c>
@@ -28832,7 +28832,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:65">
       <c r="A47" s="6" t="s">
         <v>141</v>
       </c>
@@ -28989,7 +28989,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="48" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:65">
       <c r="A48" s="6" t="s">
         <v>143</v>
       </c>
@@ -29146,7 +29146,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:65">
       <c r="A49" s="6" t="s">
         <v>73</v>
       </c>
@@ -29223,7 +29223,7 @@
       <c r="BL49" s="54"/>
       <c r="BM49" s="54"/>
     </row>
-    <row r="50" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:65">
       <c r="A50" s="6" t="s">
         <v>65</v>
       </c>
@@ -29300,7 +29300,7 @@
       <c r="BL50" s="54"/>
       <c r="BM50" s="54"/>
     </row>
-    <row r="51" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:65">
       <c r="A51" s="1" t="s">
         <v>18</v>
       </c>
@@ -29369,7 +29369,7 @@
       <c r="BL51" s="53"/>
       <c r="BM51" s="34"/>
     </row>
-    <row r="52" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:65">
       <c r="A52" s="6" t="s">
         <v>19</v>
       </c>
@@ -29448,7 +29448,7 @@
       <c r="BL52" s="25"/>
       <c r="BM52" s="25"/>
     </row>
-    <row r="53" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:65">
       <c r="A53" s="6" t="s">
         <v>22</v>
       </c>
@@ -29533,7 +29533,7 @@
       <c r="BL53" s="25"/>
       <c r="BM53" s="25"/>
     </row>
-    <row r="54" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:65">
       <c r="A54" s="6" t="s">
         <v>11</v>
       </c>
@@ -29614,7 +29614,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:65">
       <c r="H56" s="13" t="s">
         <v>30</v>
       </c>
@@ -29622,7 +29622,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="58" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:65">
       <c r="AR58" s="19" t="s">
         <v>28</v>
       </c>
@@ -29660,36 +29660,36 @@
       <selection pane="bottomRight" activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.140625" customWidth="1"/>
+    <col min="6" max="6" width="3.1640625" customWidth="1"/>
     <col min="7" max="14" width="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="3.7109375" customWidth="1"/>
+    <col min="15" max="15" width="3.6640625" customWidth="1"/>
     <col min="16" max="21" width="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="3.5703125" customWidth="1"/>
+    <col min="22" max="22" width="3.5" customWidth="1"/>
     <col min="23" max="26" width="3" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="3.85546875" customWidth="1"/>
+    <col min="27" max="27" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="3.83203125" customWidth="1"/>
     <col min="29" max="36" width="3" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="3.33203125" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="3" customWidth="1"/>
     <col min="39" max="44" width="3" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="3.85546875" customWidth="1"/>
+    <col min="45" max="45" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="3.83203125" customWidth="1"/>
     <col min="47" max="55" width="3" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="3.5703125" customWidth="1"/>
+    <col min="56" max="56" width="3.5" customWidth="1"/>
     <col min="57" max="73" width="3" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="3.5703125" customWidth="1"/>
-    <col min="75" max="75" width="3.28515625" customWidth="1"/>
-    <col min="76" max="76" width="11.42578125" customWidth="1"/>
+    <col min="74" max="74" width="3.5" customWidth="1"/>
+    <col min="75" max="75" width="3.33203125" customWidth="1"/>
+    <col min="76" max="76" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:75">
       <c r="A1" s="41" t="s">
         <v>25</v>
       </c>
@@ -29758,7 +29758,7 @@
       <c r="BL1" s="6"/>
       <c r="BM1" s="6"/>
     </row>
-    <row r="2" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:75">
       <c r="A2" s="41"/>
       <c r="B2" s="41"/>
       <c r="C2" s="41"/>
@@ -29851,7 +29851,7 @@
       <c r="BL2" s="6"/>
       <c r="BM2" s="6"/>
     </row>
-    <row r="3" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:75">
       <c r="A3" s="41"/>
       <c r="B3" s="41"/>
       <c r="C3" s="41"/>
@@ -29944,7 +29944,7 @@
       <c r="BL3" s="6"/>
       <c r="BM3" s="6"/>
     </row>
-    <row r="4" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:75">
       <c r="A4" s="23"/>
       <c r="B4" s="23"/>
       <c r="C4" s="23"/>
@@ -30023,7 +30023,7 @@
       <c r="BL4" s="6"/>
       <c r="BM4" s="6"/>
     </row>
-    <row r="6" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:75">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -30108,7 +30108,7 @@
       <c r="BV6" s="55"/>
       <c r="BW6" s="55"/>
     </row>
-    <row r="7" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:75">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -30335,7 +30335,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:75">
       <c r="A8" s="44" t="s">
         <v>5</v>
       </c>
@@ -30411,7 +30411,7 @@
       <c r="BS8" s="9"/>
       <c r="BT8" s="9"/>
     </row>
-    <row r="9" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:75">
       <c r="A9" s="5" t="s">
         <v>113</v>
       </c>
@@ -30493,7 +30493,7 @@
       <c r="BS9" s="9"/>
       <c r="BT9" s="9"/>
     </row>
-    <row r="10" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:75">
       <c r="A10" s="5" t="s">
         <v>115</v>
       </c>
@@ -30575,7 +30575,7 @@
       <c r="BS10" s="9"/>
       <c r="BT10" s="9"/>
     </row>
-    <row r="11" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:75">
       <c r="A11" s="5" t="s">
         <v>117</v>
       </c>
@@ -30657,7 +30657,7 @@
       <c r="BS11" s="9"/>
       <c r="BT11" s="9"/>
     </row>
-    <row r="12" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:75">
       <c r="A12" s="5" t="s">
         <v>119</v>
       </c>
@@ -30739,7 +30739,7 @@
       <c r="BS12" s="9"/>
       <c r="BT12" s="9"/>
     </row>
-    <row r="13" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:75">
       <c r="A13" s="5" t="s">
         <v>121</v>
       </c>
@@ -30821,7 +30821,7 @@
       <c r="BS13" s="9"/>
       <c r="BT13" s="9"/>
     </row>
-    <row r="14" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:75">
       <c r="A14" s="5" t="s">
         <v>94</v>
       </c>
@@ -30903,7 +30903,7 @@
       <c r="BS14" s="9"/>
       <c r="BT14" s="9"/>
     </row>
-    <row r="15" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:75">
       <c r="A15" s="5" t="s">
         <v>96</v>
       </c>
@@ -30989,7 +30989,7 @@
       <c r="BS15" s="9"/>
       <c r="BT15" s="9"/>
     </row>
-    <row r="16" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:75">
       <c r="A16" s="5" t="s">
         <v>90</v>
       </c>
@@ -31071,7 +31071,7 @@
       <c r="BS16" s="9"/>
       <c r="BT16" s="9"/>
     </row>
-    <row r="17" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:72">
       <c r="A17" s="5" t="s">
         <v>92</v>
       </c>
@@ -31153,7 +31153,7 @@
       <c r="BS17" s="9"/>
       <c r="BT17" s="9"/>
     </row>
-    <row r="18" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:72">
       <c r="A18" s="5" t="s">
         <v>53</v>
       </c>
@@ -31245,7 +31245,7 @@
       <c r="BS18" s="9"/>
       <c r="BT18" s="9"/>
     </row>
-    <row r="19" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:72">
       <c r="A19" s="5" t="s">
         <v>52</v>
       </c>
@@ -31333,7 +31333,7 @@
       <c r="BS19" s="9"/>
       <c r="BT19" s="9"/>
     </row>
-    <row r="20" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:72">
       <c r="A20" s="5" t="s">
         <v>57</v>
       </c>
@@ -31415,7 +31415,7 @@
       <c r="BS20" s="9"/>
       <c r="BT20" s="9"/>
     </row>
-    <row r="21" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:72">
       <c r="A21" s="5" t="s">
         <v>55</v>
       </c>
@@ -31497,7 +31497,7 @@
       <c r="BS21" s="9"/>
       <c r="BT21" s="9"/>
     </row>
-    <row r="22" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:72">
       <c r="A22" s="5" t="s">
         <v>123</v>
       </c>
@@ -31579,7 +31579,7 @@
       <c r="BS22" s="9"/>
       <c r="BT22" s="9"/>
     </row>
-    <row r="23" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:72">
       <c r="A23" s="5" t="s">
         <v>124</v>
       </c>
@@ -31667,7 +31667,7 @@
       <c r="BS23" s="9"/>
       <c r="BT23" s="9"/>
     </row>
-    <row r="24" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:72">
       <c r="A24" s="5" t="s">
         <v>125</v>
       </c>
@@ -31749,7 +31749,7 @@
       <c r="BS24" s="9"/>
       <c r="BT24" s="9"/>
     </row>
-    <row r="25" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:72">
       <c r="A25" s="5" t="s">
         <v>127</v>
       </c>
@@ -31831,7 +31831,7 @@
       <c r="BS25" s="9"/>
       <c r="BT25" s="9"/>
     </row>
-    <row r="26" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:72">
       <c r="A26" s="5" t="s">
         <v>88</v>
       </c>
@@ -31913,7 +31913,7 @@
       <c r="BS26" s="9"/>
       <c r="BT26" s="9"/>
     </row>
-    <row r="27" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:72">
       <c r="A27" s="5" t="s">
         <v>59</v>
       </c>
@@ -31995,7 +31995,7 @@
       <c r="BS27" s="9"/>
       <c r="BT27" s="9"/>
     </row>
-    <row r="28" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:72">
       <c r="A28" s="5" t="s">
         <v>61</v>
       </c>
@@ -32077,7 +32077,7 @@
       <c r="BS28" s="9"/>
       <c r="BT28" s="9"/>
     </row>
-    <row r="29" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:72">
       <c r="A29" s="5" t="s">
         <v>130</v>
       </c>
@@ -32169,7 +32169,7 @@
       <c r="BS29" s="9"/>
       <c r="BT29" s="9"/>
     </row>
-    <row r="30" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:72">
       <c r="A30" s="5" t="s">
         <v>63</v>
       </c>
@@ -32251,7 +32251,7 @@
       <c r="BS30" s="9"/>
       <c r="BT30" s="9"/>
     </row>
-    <row r="31" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:72">
       <c r="A31" s="5" t="s">
         <v>134</v>
       </c>
@@ -32343,7 +32343,7 @@
       <c r="BS31" s="9"/>
       <c r="BT31" s="9"/>
     </row>
-    <row r="32" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:72">
       <c r="A32" s="5" t="s">
         <v>89</v>
       </c>
@@ -32435,7 +32435,7 @@
       <c r="BS32" s="9"/>
       <c r="BT32" s="9"/>
     </row>
-    <row r="33" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:72">
       <c r="A33" s="1" t="s">
         <v>13</v>
       </c>
@@ -32511,7 +32511,7 @@
       <c r="BS33" s="9"/>
       <c r="BT33" s="9"/>
     </row>
-    <row r="34" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:72">
       <c r="A34" s="6" t="s">
         <v>146</v>
       </c>
@@ -32667,7 +32667,7 @@
       <c r="BS34" s="9"/>
       <c r="BT34" s="9"/>
     </row>
-    <row r="35" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:72">
       <c r="A35" s="6" t="s">
         <v>154</v>
       </c>
@@ -32823,7 +32823,7 @@
       <c r="BS35" s="9"/>
       <c r="BT35" s="9"/>
     </row>
-    <row r="36" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:72">
       <c r="A36" s="6" t="s">
         <v>98</v>
       </c>
@@ -32949,7 +32949,7 @@
       <c r="BS36" s="9"/>
       <c r="BT36" s="9"/>
     </row>
-    <row r="37" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:72">
       <c r="A37" s="6" t="s">
         <v>100</v>
       </c>
@@ -33075,7 +33075,7 @@
       <c r="BS37" s="9"/>
       <c r="BT37" s="9"/>
     </row>
-    <row r="38" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:72">
       <c r="A38" s="6" t="s">
         <v>102</v>
       </c>
@@ -33201,7 +33201,7 @@
       <c r="BS38" s="9"/>
       <c r="BT38" s="9"/>
     </row>
-    <row r="39" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:72">
       <c r="A39" s="6" t="s">
         <v>65</v>
       </c>
@@ -33285,7 +33285,7 @@
       <c r="BS39" s="50"/>
       <c r="BT39" s="51"/>
     </row>
-    <row r="40" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:72">
       <c r="A40" s="6" t="s">
         <v>67</v>
       </c>
@@ -33369,7 +33369,7 @@
       <c r="BS40" s="50"/>
       <c r="BT40" s="51"/>
     </row>
-    <row r="41" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:72">
       <c r="A41" s="6" t="s">
         <v>69</v>
       </c>
@@ -33453,7 +33453,7 @@
       <c r="BS41" s="50"/>
       <c r="BT41" s="51"/>
     </row>
-    <row r="42" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:72">
       <c r="A42" s="6" t="s">
         <v>136</v>
       </c>
@@ -33585,7 +33585,7 @@
       <c r="BS42" s="9"/>
       <c r="BT42" s="9"/>
     </row>
-    <row r="43" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:72">
       <c r="A43" s="6" t="s">
         <v>71</v>
       </c>
@@ -33669,7 +33669,7 @@
       <c r="BS43" s="50"/>
       <c r="BT43" s="51"/>
     </row>
-    <row r="44" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:72">
       <c r="A44" s="6" t="s">
         <v>138</v>
       </c>
@@ -33785,7 +33785,7 @@
       <c r="BS44" s="9"/>
       <c r="BT44" s="9"/>
     </row>
-    <row r="45" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:72">
       <c r="A45" s="6" t="s">
         <v>139</v>
       </c>
@@ -33901,7 +33901,7 @@
       <c r="BS45" s="9"/>
       <c r="BT45" s="9"/>
     </row>
-    <row r="46" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:72">
       <c r="A46" s="6" t="s">
         <v>103</v>
       </c>
@@ -34057,7 +34057,7 @@
       <c r="BS46" s="9"/>
       <c r="BT46" s="9"/>
     </row>
-    <row r="47" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:72">
       <c r="A47" s="6" t="s">
         <v>141</v>
       </c>
@@ -34189,7 +34189,7 @@
       <c r="BS47" s="9"/>
       <c r="BT47" s="9"/>
     </row>
-    <row r="48" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:72">
       <c r="A48" s="6" t="s">
         <v>143</v>
       </c>
@@ -34321,7 +34321,7 @@
       <c r="BS48" s="9"/>
       <c r="BT48" s="9"/>
     </row>
-    <row r="49" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:72">
       <c r="A49" s="6" t="s">
         <v>73</v>
       </c>
@@ -34405,7 +34405,7 @@
       <c r="BS49" s="50"/>
       <c r="BT49" s="51"/>
     </row>
-    <row r="50" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:72">
       <c r="A50" s="6" t="s">
         <v>65</v>
       </c>
@@ -34489,7 +34489,7 @@
       <c r="BS50" s="50"/>
       <c r="BT50" s="51"/>
     </row>
-    <row r="51" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:72">
       <c r="A51" s="1" t="s">
         <v>18</v>
       </c>
@@ -34565,7 +34565,7 @@
       <c r="BS51" s="9"/>
       <c r="BT51" s="9"/>
     </row>
-    <row r="52" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:72">
       <c r="A52" s="6" t="s">
         <v>19</v>
       </c>
@@ -34653,7 +34653,7 @@
       <c r="BS52" s="9"/>
       <c r="BT52" s="9"/>
     </row>
-    <row r="53" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:72">
       <c r="A53" s="6" t="s">
         <v>22</v>
       </c>
@@ -34741,7 +34741,7 @@
       <c r="BS53" s="9"/>
       <c r="BT53" s="9"/>
     </row>
-    <row r="54" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:72">
       <c r="A54" s="6" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
fix: make available people a computed property and only show workdays
</commit_message>
<xml_diff>
--- a/SampleData/02_Anwesenheit/Urlaubs-Schulkalender_23.xlsx
+++ b/SampleData/02_Anwesenheit/Urlaubs-Schulkalender_23.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrick/dev/Web Projects/MurrChooser/SampleData/02_Anwesenheit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A3E5C2-1C92-9648-BE8A-62B1E8AE2F5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E95DDB8-F8C1-A847-BA9B-F4DC90CC0541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Januar Februar 2023" sheetId="8" r:id="rId1"/>
@@ -1361,11 +1361,11 @@
   </sheetPr>
   <dimension ref="A1:BK64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" ySplit="8" topLeftCell="N18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="A33" sqref="A33:XFD33"/>
+      <selection pane="bottomRight" activeCell="BK7" sqref="BK7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1829,154 +1829,154 @@
         <v>44448</v>
       </c>
       <c r="N7" s="24">
-        <v>44449</v>
+        <v>44936</v>
       </c>
       <c r="O7" s="24">
-        <v>44450</v>
+        <v>44937</v>
       </c>
       <c r="P7" s="24">
-        <v>44451</v>
+        <v>44938</v>
       </c>
       <c r="Q7" s="24">
-        <v>44452</v>
+        <v>44939</v>
       </c>
       <c r="R7" s="24">
-        <v>44453</v>
+        <v>44940</v>
       </c>
       <c r="S7" s="24">
-        <v>44454</v>
+        <v>44941</v>
       </c>
       <c r="T7" s="24">
-        <v>44455</v>
+        <v>44942</v>
       </c>
       <c r="U7" s="24">
-        <v>44456</v>
+        <v>44943</v>
       </c>
       <c r="V7" s="24">
-        <v>44457</v>
+        <v>44944</v>
       </c>
       <c r="W7" s="24">
-        <v>44458</v>
+        <v>44945</v>
       </c>
       <c r="X7" s="24">
-        <v>44459</v>
+        <v>44946</v>
       </c>
       <c r="Y7" s="24">
-        <v>44460</v>
+        <v>44947</v>
       </c>
       <c r="Z7" s="24">
-        <v>44461</v>
+        <v>44948</v>
       </c>
       <c r="AA7" s="24">
-        <v>44462</v>
+        <v>44949</v>
       </c>
       <c r="AB7" s="24">
-        <v>44463</v>
+        <v>44950</v>
       </c>
       <c r="AC7" s="24">
-        <v>44464</v>
+        <v>44951</v>
       </c>
       <c r="AD7" s="24">
-        <v>44465</v>
+        <v>44952</v>
       </c>
       <c r="AE7" s="24">
-        <v>44466</v>
+        <v>44953</v>
       </c>
       <c r="AF7" s="24">
-        <v>44467</v>
+        <v>44954</v>
       </c>
       <c r="AG7" s="24">
-        <v>44468</v>
+        <v>44955</v>
       </c>
       <c r="AH7" s="24">
-        <v>44469</v>
+        <v>44956</v>
       </c>
       <c r="AI7" s="24">
-        <v>31</v>
+        <v>44957</v>
       </c>
       <c r="AJ7" s="24">
-        <v>44470</v>
+        <v>44958</v>
       </c>
       <c r="AK7" s="24">
-        <v>44471</v>
+        <v>44959</v>
       </c>
       <c r="AL7" s="24">
-        <v>44472</v>
+        <v>44960</v>
       </c>
       <c r="AM7" s="24">
-        <v>44473</v>
+        <v>44961</v>
       </c>
       <c r="AN7" s="24">
-        <v>44474</v>
+        <v>44962</v>
       </c>
       <c r="AO7" s="24">
-        <v>44475</v>
+        <v>44963</v>
       </c>
       <c r="AP7" s="24">
-        <v>44476</v>
+        <v>44964</v>
       </c>
       <c r="AQ7" s="24">
-        <v>44477</v>
+        <v>44965</v>
       </c>
       <c r="AR7" s="24">
-        <v>44478</v>
+        <v>44966</v>
       </c>
       <c r="AS7" s="24">
-        <v>44479</v>
+        <v>44967</v>
       </c>
       <c r="AT7" s="24">
-        <v>44480</v>
+        <v>44968</v>
       </c>
       <c r="AU7" s="24">
-        <v>44481</v>
+        <v>44969</v>
       </c>
       <c r="AV7" s="24">
-        <v>44482</v>
+        <v>44970</v>
       </c>
       <c r="AW7" s="24">
-        <v>44483</v>
+        <v>44971</v>
       </c>
       <c r="AX7" s="24">
-        <v>44484</v>
+        <v>44972</v>
       </c>
       <c r="AY7" s="24">
-        <v>44485</v>
+        <v>44973</v>
       </c>
       <c r="AZ7" s="24">
-        <v>44486</v>
+        <v>44974</v>
       </c>
       <c r="BA7" s="24">
-        <v>44487</v>
+        <v>44975</v>
       </c>
       <c r="BB7" s="24">
-        <v>44488</v>
+        <v>44976</v>
       </c>
       <c r="BC7" s="24">
-        <v>44489</v>
+        <v>44977</v>
       </c>
       <c r="BD7" s="24">
-        <v>44490</v>
+        <v>44978</v>
       </c>
       <c r="BE7" s="24">
-        <v>44491</v>
+        <v>44979</v>
       </c>
       <c r="BF7" s="24">
-        <v>44492</v>
+        <v>44980</v>
       </c>
       <c r="BG7" s="24">
-        <v>44493</v>
+        <v>44981</v>
       </c>
       <c r="BH7" s="24">
-        <v>44494</v>
+        <v>44982</v>
       </c>
       <c r="BI7" s="24">
-        <v>44495</v>
+        <v>44983</v>
       </c>
       <c r="BJ7" s="24">
-        <v>44496</v>
+        <v>44984</v>
       </c>
       <c r="BK7" s="24">
-        <v>44497</v>
+        <v>44985</v>
       </c>
     </row>
     <row r="8" spans="1:63">
@@ -13563,11 +13563,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:BM56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="8" topLeftCell="E9" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="4" ySplit="8" topLeftCell="E28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="BM7" sqref="BM7"/>
+      <selection pane="bottomRight" activeCell="AN54" sqref="AN54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>